<commit_message>
Criada classe responsável por importar os dados enviados no Excel. As instruções para importação foram removidas do controller e adicionados nesta classe
</commit_message>
<xml_diff>
--- a/app/storage/import/products_teste_webdev_leroy.xlsx
+++ b/app/storage/import/products_teste_webdev_leroy.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Ferramentas</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>free_shipping</t>
+  </si>
+  <si>
+    <t>Apple Trackpad</t>
+  </si>
+  <si>
+    <t>Melhor trackpad do mundo</t>
   </si>
 </sst>
 </file>
@@ -150,8 +156,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,13 +171,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,9 +479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
@@ -612,6 +624,26 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>1011</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>257.55</v>
+      </c>
+      <c r="F8" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>